<commit_message>
issue with not decting empty zones
</commit_message>
<xml_diff>
--- a/outputs/results/recordings_summary.xlsx
+++ b/outputs/results/recordings_summary.xlsx
@@ -543,16 +543,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
         <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -565,16 +565,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>100</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="4">
@@ -590,13 +590,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -612,13 +612,13 @@
         <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>100</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="6">
@@ -634,13 +634,13 @@
         <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="7">
@@ -656,13 +656,13 @@
         <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
@@ -675,16 +675,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>